<commit_message>
- Agregado datos de pruebas.- - Se ha agregado la posibilidad de que el recalcular % se puede escoger entre LCL y VST
</commit_message>
<xml_diff>
--- a/Otras cosas/Pronósticos - Tenis/Datos.xlsx
+++ b/Otras cosas/Pronósticos - Tenis/Datos.xlsx
@@ -1,10 +1,11 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F12BE2-8ED7-4C45-BC83-430E3AC94F5F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="5" r:id="rId1"/>
@@ -14,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="44" uniqueCount="43">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="115">
   <si>
     <t>//---------PROBABILIDAD DE VICTORIA</t>
   </si>
@@ -143,13 +144,229 @@
   </si>
   <si>
     <t>Prob OVER/UNDER de 40.5 -&gt;&gt; ,00% - 100,00%</t>
+  </si>
+  <si>
+    <t>Jared Donaldson</t>
+  </si>
+  <si>
+    <t>vs</t>
+  </si>
+  <si>
+    <t>Denis Shapovalov</t>
+  </si>
+  <si>
+    <t>-&gt;&gt; 1281 vs 1219</t>
+  </si>
+  <si>
+    <t>-&gt;&gt; 51,24%</t>
+  </si>
+  <si>
+    <t>-&gt;&gt; 48,76%</t>
+  </si>
+  <si>
+    <t>RESULTADO 2-0 -&gt;&gt; 26,00%</t>
+  </si>
+  <si>
+    <t>RESULTADO 2-1 -&gt;&gt; 25,24%</t>
+  </si>
+  <si>
+    <t>RESULTADO 0-2 -&gt;&gt; 23,84%</t>
+  </si>
+  <si>
+    <t>RESULTADO 1-2 -&gt;&gt; 24,92%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 13.5 -&gt;&gt; 99,96% - ,04%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 14.5 -&gt;&gt; 99,96% - ,04%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 15.5 -&gt;&gt; 99,48% - ,52%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 16.5 -&gt;&gt; 98,72% - 1,28%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 17.5 -&gt;&gt; 95,96% - 4,04%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 18.5 -&gt;&gt; 91,44% - 8,56%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 19.5 -&gt;&gt; 84,60% - 15,40%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 20.5 -&gt;&gt; 76,84% - 23,16%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 21.5 -&gt;&gt; 71,48% - 28,52%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 22.5 -&gt;&gt; 62,60% - 37,40%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 23.5 -&gt;&gt; 58,12% - 41,88%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 24.5 -&gt;&gt; 57,48% - 42,52%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 25.5 -&gt;&gt; 54,24% - 45,76%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 26.5 -&gt;&gt; 46,68% - 53,32%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 27.5 -&gt;&gt; 43,88% - 56,12%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 28.5 -&gt;&gt; 40,56% - 59,44%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 29.5 -&gt;&gt; 36,44% - 63,56%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 30.5 -&gt;&gt; 31,28% - 68,72%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 31.5 -&gt;&gt; 24,24% - 75,76%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 32.5 -&gt;&gt; 16,28% - 83,72%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 33.5 -&gt;&gt; 11,76% - 88,24%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 34.5 -&gt;&gt; 8,36% - 91,64%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 35.5 -&gt;&gt; 4,24% - 95,76%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 36.5 -&gt;&gt; ,84% - 99,16%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 37.5 -&gt;&gt; ,76% - 99,24%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 38.5 -&gt;&gt; ,36% - 99,64%</t>
+  </si>
+  <si>
+    <t>@2,50/@1,50</t>
+  </si>
+  <si>
+    <t>-&gt;&gt; 571 vs 429</t>
+  </si>
+  <si>
+    <t>-&gt;&gt; 57,10%</t>
+  </si>
+  <si>
+    <t>-&gt;&gt; 42,90%</t>
+  </si>
+  <si>
+    <t>RESULTADO 2-0 -&gt;&gt; 30,30%</t>
+  </si>
+  <si>
+    <t>RESULTADO 2-1 -&gt;&gt; 26,80%</t>
+  </si>
+  <si>
+    <t>RESULTADO 0-2 -&gt;&gt; 19,90%</t>
+  </si>
+  <si>
+    <t>RESULTADO 1-2 -&gt;&gt; 23,00%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 14.5 -&gt;&gt; 100,00% - ,00%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 15.5 -&gt;&gt; 99,60% - ,40%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 16.5 -&gt;&gt; 99,20% - ,80%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 17.5 -&gt;&gt; 97,30% - 2,70%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 18.5 -&gt;&gt; 94,50% - 5,50%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 19.5 -&gt;&gt; 88,40% - 11,60%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 20.5 -&gt;&gt; 80,70% - 19,30%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 21.5 -&gt;&gt; 77,00% - 23,00%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 22.5 -&gt;&gt; 68,00% - 32,00%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 23.5 -&gt;&gt; 64,30% - 35,70%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 24.5 -&gt;&gt; 63,40% - 36,60%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 25.5 -&gt;&gt; 59,30% - 40,70%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 26.5 -&gt;&gt; 47,40% - 52,60%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 27.5 -&gt;&gt; 45,40% - 54,60%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 28.5 -&gt;&gt; 42,90% - 57,10%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 29.5 -&gt;&gt; 39,60% - 60,40%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 30.5 -&gt;&gt; 35,00% - 65,00%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 31.5 -&gt;&gt; 28,90% - 71,10%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 32.5 -&gt;&gt; 22,80% - 77,20%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 33.5 -&gt;&gt; 16,90% - 83,10%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 34.5 -&gt;&gt; 13,50% - 86,50%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 35.5 -&gt;&gt; 8,00% - 92,00%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 36.5 -&gt;&gt; 2,40% - 97,60%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 37.5 -&gt;&gt; 1,70% - 98,30%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 38.5 -&gt;&gt; ,60% - 99,40%</t>
+  </si>
+  <si>
+    <t>Gilles Simon</t>
+  </si>
+  <si>
+    <t>Leonardo Mayer</t>
+  </si>
+  <si>
+    <t>@1,72/@2.00</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <fonts count="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -158,12 +375,18 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="1" tint="0.249977111117893"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -178,14 +401,24 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
+      <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
+    </ext>
+    <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{9260A510-F301-46a8-8635-F512D64BE5F5}">
+      <x15:timelineStyles defaultTimelineStyle="TimeSlicerStyleLight1"/>
+    </ext>
+  </extLst>
 </styleSheet>
 </file>
 
@@ -206,7 +439,13 @@
     </xdr:to>
     <xdr:pic>
       <xdr:nvPicPr>
-        <xdr:cNvPr id="1025" name="Picture 1"/>
+        <xdr:cNvPr id="1025" name="Picture 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
         <xdr:cNvPicPr>
           <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
         </xdr:cNvPicPr>
@@ -284,7 +523,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria"/>
+        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -316,9 +555,27 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri"/>
+        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -350,6 +607,24 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
+        <a:font script="Geor" typeface="Sylfaen"/>
+        <a:font script="Armn" typeface="Arial"/>
+        <a:font script="Bugi" typeface="Leelawadee UI"/>
+        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
+        <a:font script="Java" typeface="Javanese Text"/>
+        <a:font script="Lisu" typeface="Segoe UI"/>
+        <a:font script="Mymr" typeface="Myanmar Text"/>
+        <a:font script="Nkoo" typeface="Ebrima"/>
+        <a:font script="Olck" typeface="Nirmala UI"/>
+        <a:font script="Osma" typeface="Ebrima"/>
+        <a:font script="Phag" typeface="Phagspa"/>
+        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
+        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
+        <a:font script="Syre" typeface="Estrangelo Edessa"/>
+        <a:font script="Sora" typeface="Nirmala UI"/>
+        <a:font script="Tale" typeface="Microsoft Tai Le"/>
+        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
+        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -525,21 +800,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="B5:E49"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A5:Q149"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G5" sqref="G5"/>
+      <selection activeCell="G104" sqref="G104"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="5" spans="2:5">
+    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:5">
+    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -547,7 +822,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:5">
+    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -555,7 +830,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:5">
+    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -563,188 +838,682 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:5">
+    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:5">
+    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:5">
+    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:5">
+    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:5">
+    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:5">
+    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:2">
+    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:2">
+    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="2:2">
+    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="2:2">
+    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:2">
+    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="2:2">
+    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="2:2">
+    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:2">
+    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="2:2">
+    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="2:2">
+    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="2:2">
+    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="2:2">
+    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="2:2">
+    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="2:2">
+    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="2:2">
+    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="2:2">
+    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="2:2">
+    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:2">
+    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B36" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="2:2">
+    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B37" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="2:2">
+    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B38" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="2:2">
+    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="2:2">
+    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B40" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="2:2">
+    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="2:2">
+    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B42" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="2:2">
+    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="2:2">
+    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B44" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="2:2">
+    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B45" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="2:2">
+    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B46" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="2:2">
+    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B47" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="2:2">
+    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
       <c r="B48" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="2:2">
+    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B49" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A51" s="1"/>
+      <c r="B51" s="1"/>
+      <c r="C51" s="1"/>
+      <c r="D51" s="1"/>
+      <c r="E51" s="1"/>
+      <c r="F51" s="1"/>
+      <c r="G51" s="1"/>
+      <c r="H51" s="1"/>
+      <c r="I51" s="1"/>
+      <c r="J51" s="1"/>
+      <c r="K51" s="1"/>
+      <c r="L51" s="1"/>
+      <c r="M51" s="1"/>
+      <c r="N51" s="1"/>
+      <c r="O51" s="1"/>
+      <c r="P51" s="1"/>
+      <c r="Q51" s="1"/>
+    </row>
+    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B53" t="s">
+        <v>43</v>
+      </c>
+      <c r="D53" t="s">
+        <v>44</v>
+      </c>
+      <c r="E53" t="s">
+        <v>45</v>
+      </c>
+      <c r="G53" s="2" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B55" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B56" t="s">
+        <v>1</v>
+      </c>
+      <c r="E56" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B57" t="s">
+        <v>3</v>
+      </c>
+      <c r="D57" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B58" t="s">
+        <v>5</v>
+      </c>
+      <c r="C58" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B59" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B62" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B63" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B64" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B65" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B66" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B67" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B70" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B71" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B72" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B73" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B74" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B75" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B76" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B77" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B78" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B79" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B80" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B81" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B82" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B83" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B84" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B85" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B86" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B87" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B88" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B89" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B90" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B91" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B92" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B93" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B94" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B95" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B96" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B97" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B98" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B99" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="A101" s="1"/>
+      <c r="B101" s="1"/>
+      <c r="C101" s="1"/>
+      <c r="D101" s="1"/>
+      <c r="E101" s="1"/>
+      <c r="F101" s="1"/>
+      <c r="G101" s="1"/>
+      <c r="H101" s="1"/>
+      <c r="I101" s="1"/>
+      <c r="J101" s="1"/>
+      <c r="K101" s="1"/>
+      <c r="L101" s="1"/>
+      <c r="M101" s="1"/>
+      <c r="N101" s="1"/>
+      <c r="O101" s="1"/>
+      <c r="P101" s="1"/>
+      <c r="Q101" s="1"/>
+    </row>
+    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B103" t="s">
+        <v>112</v>
+      </c>
+      <c r="D103" t="s">
+        <v>44</v>
+      </c>
+      <c r="E103" t="s">
+        <v>113</v>
+      </c>
+      <c r="G103" s="2" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B105" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B106" t="s">
+        <v>1</v>
+      </c>
+      <c r="E106" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B107" t="s">
+        <v>3</v>
+      </c>
+      <c r="D107" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B108" t="s">
+        <v>5</v>
+      </c>
+      <c r="C108" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B109" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="B112" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B113" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B114" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B115" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B116" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B117" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B120" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B121" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B122" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B123" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B124" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B125" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B126" t="s">
+        <v>90</v>
+      </c>
+    </row>
+    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B127" t="s">
+        <v>91</v>
+      </c>
+    </row>
+    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B128" t="s">
+        <v>92</v>
+      </c>
+    </row>
+    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B129" t="s">
+        <v>93</v>
+      </c>
+    </row>
+    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B130" t="s">
+        <v>94</v>
+      </c>
+    </row>
+    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B131" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B132" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B133" t="s">
+        <v>97</v>
+      </c>
+    </row>
+    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B134" t="s">
+        <v>98</v>
+      </c>
+    </row>
+    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B135" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B136" t="s">
+        <v>100</v>
+      </c>
+    </row>
+    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B137" t="s">
+        <v>101</v>
+      </c>
+    </row>
+    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B138" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B139" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B140" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B141" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B142" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B143" t="s">
+        <v>107</v>
+      </c>
+    </row>
+    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B144" t="s">
+        <v>108</v>
+      </c>
+    </row>
+    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B145" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B146" t="s">
+        <v>110</v>
+      </c>
+    </row>
+    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B147" t="s">
+        <v>111</v>
+      </c>
+    </row>
+    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B148" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+      <c r="B149" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Actualizamos excel de datos
</commit_message>
<xml_diff>
--- a/Otras cosas/Pronósticos - Tenis/Datos.xlsx
+++ b/Otras cosas/Pronósticos - Tenis/Datos.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B1F12BE2-8ED7-4C45-BC83-430E3AC94F5F}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E630AA61-CD60-44C3-83F0-7B42F9B65C80}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="116">
   <si>
     <t>//---------PROBABILIDAD DE VICTORIA</t>
   </si>
@@ -360,6 +360,9 @@
   </si>
   <si>
     <t>@1,72/@2.00</t>
+  </si>
+  <si>
+    <t>4-6 6-7</t>
   </si>
 </sst>
 </file>
@@ -803,8 +806,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A5:Q149"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="G104" sqref="G104"/>
+    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="H105" sqref="H105"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1303,6 +1306,11 @@
         <v>114</v>
       </c>
     </row>
+    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+      <c r="G104" t="s">
+        <v>115</v>
+      </c>
+    </row>
     <row r="105" spans="1:17" x14ac:dyDescent="0.25">
       <c r="B105" t="s">
         <v>0</v>

</xml_diff>

<commit_message>
Datos actualizados con 3 nuevas apuestas
</commit_message>
<xml_diff>
--- a/Otras cosas/Pronósticos - Tenis/Datos.xlsx
+++ b/Otras cosas/Pronósticos - Tenis/Datos.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="19330"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="4" lowestEdited="4" rupBuild="4507"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E630AA61-CD60-44C3-83F0-7B42F9B65C80}" xr6:coauthVersionLast="33" xr6:coauthVersionMax="33" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="360" yWindow="300" windowWidth="14880" windowHeight="7815"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="5" r:id="rId1"/>
@@ -15,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="141" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="274" uniqueCount="209">
   <si>
     <t>//---------PROBABILIDAD DE VICTORIA</t>
   </si>
@@ -363,13 +362,292 @@
   </si>
   <si>
     <t>4-6 6-7</t>
+  </si>
+  <si>
+    <t>-&gt;&gt; 440 vs 560</t>
+  </si>
+  <si>
+    <t>-&gt;&gt; 44,00%</t>
+  </si>
+  <si>
+    <t>-&gt;&gt; 56,00%</t>
+  </si>
+  <si>
+    <t>RESULTADO 2-0 -&gt;&gt; 20,10%</t>
+  </si>
+  <si>
+    <t>RESULTADO 2-1 -&gt;&gt; 23,90%</t>
+  </si>
+  <si>
+    <t>RESULTADO 0-2 -&gt;&gt; 29,50%</t>
+  </si>
+  <si>
+    <t>RESULTADO 1-2 -&gt;&gt; 26,50%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 15.5 -&gt;&gt; 99,30% - ,70%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 16.5 -&gt;&gt; 97,60% - 2,40%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 17.5 -&gt;&gt; 94,20% - 5,80%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 18.5 -&gt;&gt; 88,80% - 11,20%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 19.5 -&gt;&gt; 82,20% - 17,80%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 20.5 -&gt;&gt; 75,40% - 24,60%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 21.5 -&gt;&gt; 70,80% - 29,20%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 22.5 -&gt;&gt; 62,30% - 37,70%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 23.5 -&gt;&gt; 57,20% - 42,80%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 24.5 -&gt;&gt; 56,70% - 43,30%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 25.5 -&gt;&gt; 53,40% - 46,60%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 26.5 -&gt;&gt; 45,10% - 54,90%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 27.5 -&gt;&gt; 42,10% - 57,90%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 28.5 -&gt;&gt; 37,90% - 62,10%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 29.5 -&gt;&gt; 31,20% - 68,80%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 30.5 -&gt;&gt; 26,90% - 73,10%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 31.5 -&gt;&gt; 19,30% - 80,70%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 32.5 -&gt;&gt; 13,20% - 86,80%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 33.5 -&gt;&gt; 9,60% - 90,40%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 34.5 -&gt;&gt; 6,60% - 93,40%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 35.5 -&gt;&gt; 3,90% - 96,10%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 36.5 -&gt;&gt; 1,40% - 98,60%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 37.5 -&gt;&gt; 1,00% - 99,00%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 38.5 -&gt;&gt; ,30% - 99,70%</t>
+  </si>
+  <si>
+    <t>-&gt;&gt; 641 vs 359</t>
+  </si>
+  <si>
+    <t>-&gt;&gt; 64,10%</t>
+  </si>
+  <si>
+    <t>-&gt;&gt; 35,90%</t>
+  </si>
+  <si>
+    <t>RESULTADO 2-0 -&gt;&gt; 34,80%</t>
+  </si>
+  <si>
+    <t>RESULTADO 2-1 -&gt;&gt; 29,30%</t>
+  </si>
+  <si>
+    <t>RESULTADO 0-2 -&gt;&gt; 14,80%</t>
+  </si>
+  <si>
+    <t>RESULTADO 1-2 -&gt;&gt; 21,10%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 14.5 -&gt;&gt; 99,80% - ,20%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 15.5 -&gt;&gt; 98,90% - 1,10%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 16.5 -&gt;&gt; 96,90% - 3,10%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 17.5 -&gt;&gt; 92,20% - 7,80%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 18.5 -&gt;&gt; 86,90% - 13,10%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 19.5 -&gt;&gt; 79,50% - 20,50%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 20.5 -&gt;&gt; 72,60% - 27,40%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 21.5 -&gt;&gt; 68,90% - 31,10%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 22.5 -&gt;&gt; 61,20% - 38,80%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 23.5 -&gt;&gt; 56,50% - 43,50%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 24.5 -&gt;&gt; 54,70% - 45,30%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 25.5 -&gt;&gt; 50,60% - 49,40%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 26.5 -&gt;&gt; 44,50% - 55,50%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 27.5 -&gt;&gt; 40,80% - 59,20%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 28.5 -&gt;&gt; 36,30% - 63,70%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 29.5 -&gt;&gt; 32,40% - 67,60%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 30.5 -&gt;&gt; 27,10% - 72,90%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 31.5 -&gt;&gt; 19,70% - 80,30%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 32.5 -&gt;&gt; 13,90% - 86,10%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 33.5 -&gt;&gt; 9,20% - 90,80%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 34.5 -&gt;&gt; 6,50% - 93,50%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 35.5 -&gt;&gt; 2,90% - 97,10%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 37.5 -&gt;&gt; ,90% - 99,10%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 38.5 -&gt;&gt; ,20% - 99,80%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 41.5 -&gt;&gt; ,00% - 100,00%</t>
+  </si>
+  <si>
+    <t>-&gt;&gt; 471 vs 529</t>
+  </si>
+  <si>
+    <t>-&gt;&gt; 47,10%</t>
+  </si>
+  <si>
+    <t>-&gt;&gt; 52,90%</t>
+  </si>
+  <si>
+    <t>RESULTADO 2-0 -&gt;&gt; 22,30%</t>
+  </si>
+  <si>
+    <t>RESULTADO 2-1 -&gt;&gt; 24,80%</t>
+  </si>
+  <si>
+    <t>RESULTADO 0-2 -&gt;&gt; 26,20%</t>
+  </si>
+  <si>
+    <t>RESULTADO 1-2 -&gt;&gt; 26,70%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 15.5 -&gt;&gt; 99,50% - ,50%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 16.5 -&gt;&gt; 98,30% - 1,70%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 17.5 -&gt;&gt; 95,50% - 4,50%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 18.5 -&gt;&gt; 91,20% - 8,80%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 19.5 -&gt;&gt; 84,00% - 16,00%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 20.5 -&gt;&gt; 77,10% - 22,90%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 21.5 -&gt;&gt; 72,80% - 27,20%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 22.5 -&gt;&gt; 64,20% - 35,80%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 23.5 -&gt;&gt; 60,10% - 39,90%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 24.5 -&gt;&gt; 59,60% - 40,40%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 25.5 -&gt;&gt; 56,20% - 43,80%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 26.5 -&gt;&gt; 46,60% - 53,40%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 27.5 -&gt;&gt; 44,30% - 55,70%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 28.5 -&gt;&gt; 41,10% - 58,90%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 29.5 -&gt;&gt; 38,10% - 61,90%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 30.5 -&gt;&gt; 33,40% - 66,60%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 31.5 -&gt;&gt; 26,80% - 73,20%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 32.5 -&gt;&gt; 18,60% - 81,40%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 33.5 -&gt;&gt; 12,40% - 87,60%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 34.5 -&gt;&gt; 9,10% - 90,90%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 35.5 -&gt;&gt; 4,50% - 95,50%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 36.5 -&gt;&gt; 1,80% - 98,20%</t>
+  </si>
+  <si>
+    <t>Prob OVER/UNDER de 37.5 -&gt;&gt; 1,40% - 98,60%</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+  <fonts count="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -445,7 +723,7 @@
         <xdr:cNvPr id="1025" name="Picture 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0000-000001040000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0000-000001040000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -464,6 +742,147 @@
         <a:xfrm>
           <a:off x="762000" y="381000"/>
           <a:ext cx="13315950" cy="352425"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>152</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>17</xdr:col>
+      <xdr:colOff>723900</xdr:colOff>
+      <xdr:row>153</xdr:row>
+      <xdr:rowOff>123825</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="2" name="Picture 1"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId2" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="762000" y="28956000"/>
+          <a:ext cx="12915900" cy="314325"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>202</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>381000</xdr:colOff>
+      <xdr:row>203</xdr:row>
+      <xdr:rowOff>85725</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1026" name="Picture 2"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId3" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="762000" y="38481000"/>
+          <a:ext cx="13335000" cy="276225"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:noFill/>
+        <a:ln w="1">
+          <a:noFill/>
+          <a:miter lim="800000"/>
+          <a:headEnd/>
+          <a:tailEnd type="none" w="med" len="med"/>
+        </a:ln>
+        <a:effectLst/>
+      </xdr:spPr>
+    </xdr:pic>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor editAs="oneCell">
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>253</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>333375</xdr:colOff>
+      <xdr:row>254</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:pic>
+      <xdr:nvPicPr>
+        <xdr:cNvPr id="1027" name="Picture 3"/>
+        <xdr:cNvPicPr>
+          <a:picLocks noChangeAspect="1" noChangeArrowheads="1"/>
+        </xdr:cNvPicPr>
+      </xdr:nvPicPr>
+      <xdr:blipFill>
+        <a:blip xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:embed="rId4" cstate="print"/>
+        <a:srcRect/>
+        <a:stretch>
+          <a:fillRect/>
+        </a:stretch>
+      </xdr:blipFill>
+      <xdr:spPr bwMode="auto">
+        <a:xfrm>
+          <a:off x="762000" y="48196500"/>
+          <a:ext cx="13287375" cy="266700"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
           <a:avLst/>
@@ -526,7 +945,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Cambria" panose="020F0302020204030204"/>
+        <a:latin typeface="Cambria"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -558,27 +977,9 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Times New Roman"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="ＭＳ Ｐゴシック"/>
@@ -610,24 +1011,6 @@
         <a:font script="Mong" typeface="Mongolian Baiti"/>
         <a:font script="Viet" typeface="Arial"/>
         <a:font script="Uigh" typeface="Microsoft Uighur"/>
-        <a:font script="Geor" typeface="Sylfaen"/>
-        <a:font script="Armn" typeface="Arial"/>
-        <a:font script="Bugi" typeface="Leelawadee UI"/>
-        <a:font script="Bopo" typeface="Microsoft JhengHei"/>
-        <a:font script="Java" typeface="Javanese Text"/>
-        <a:font script="Lisu" typeface="Segoe UI"/>
-        <a:font script="Mymr" typeface="Myanmar Text"/>
-        <a:font script="Nkoo" typeface="Ebrima"/>
-        <a:font script="Olck" typeface="Nirmala UI"/>
-        <a:font script="Osma" typeface="Ebrima"/>
-        <a:font script="Phag" typeface="Phagspa"/>
-        <a:font script="Syrn" typeface="Estrangelo Edessa"/>
-        <a:font script="Syrj" typeface="Estrangelo Edessa"/>
-        <a:font script="Syre" typeface="Estrangelo Edessa"/>
-        <a:font script="Sora" typeface="Nirmala UI"/>
-        <a:font script="Tale" typeface="Microsoft Tai Le"/>
-        <a:font script="Talu" typeface="Microsoft New Tai Lue"/>
-        <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
     <a:fmtScheme name="Office">
@@ -803,21 +1186,21 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A5:Q149"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <dimension ref="A5:Q300"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A110" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="H105" sqref="H105"/>
+    <sheetView tabSelected="1" topLeftCell="A236" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="N258" sqref="N258"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15"/>
   <sheetData>
-    <row r="5" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="5" spans="2:5">
       <c r="B5" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="6" spans="2:5">
       <c r="B6" t="s">
         <v>1</v>
       </c>
@@ -825,7 +1208,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="7" spans="2:5">
       <c r="B7" t="s">
         <v>3</v>
       </c>
@@ -833,7 +1216,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="8" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="8" spans="2:5">
       <c r="B8" t="s">
         <v>5</v>
       </c>
@@ -841,192 +1224,192 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="9" spans="2:5">
       <c r="B9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="12" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="12" spans="2:5">
       <c r="B12" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="13" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="13" spans="2:5">
       <c r="B13" t="s">
         <v>9</v>
       </c>
     </row>
-    <row r="14" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="14" spans="2:5">
       <c r="B14" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="15" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="15" spans="2:5">
       <c r="B15" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="16" spans="2:5" x14ac:dyDescent="0.25">
+    <row r="16" spans="2:5">
       <c r="B16" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="17" spans="2:2">
       <c r="B17" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="20" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="20" spans="2:2">
       <c r="B20" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="21" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="21" spans="2:2">
       <c r="B21" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="22" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="22" spans="2:2">
       <c r="B22" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="23" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="23" spans="2:2">
       <c r="B23" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="24" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="24" spans="2:2">
       <c r="B24" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="25" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="25" spans="2:2">
       <c r="B25" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="26" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="26" spans="2:2">
       <c r="B26" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="27" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="27" spans="2:2">
       <c r="B27" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="28" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="28" spans="2:2">
       <c r="B28" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="29" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="29" spans="2:2">
       <c r="B29" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="30" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="30" spans="2:2">
       <c r="B30" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="31" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="31" spans="2:2">
       <c r="B31" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="32" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="32" spans="2:2">
       <c r="B32" t="s">
         <v>25</v>
       </c>
     </row>
-    <row r="33" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="33" spans="2:2">
       <c r="B33" t="s">
         <v>26</v>
       </c>
     </row>
-    <row r="34" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="34" spans="2:2">
       <c r="B34" t="s">
         <v>27</v>
       </c>
     </row>
-    <row r="35" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="35" spans="2:2">
       <c r="B35" t="s">
         <v>28</v>
       </c>
     </row>
-    <row r="36" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="36" spans="2:2">
       <c r="B36" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="37" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="37" spans="2:2">
       <c r="B37" t="s">
         <v>30</v>
       </c>
     </row>
-    <row r="38" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="38" spans="2:2">
       <c r="B38" t="s">
         <v>31</v>
       </c>
     </row>
-    <row r="39" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="39" spans="2:2">
       <c r="B39" t="s">
         <v>32</v>
       </c>
     </row>
-    <row r="40" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="40" spans="2:2">
       <c r="B40" t="s">
         <v>33</v>
       </c>
     </row>
-    <row r="41" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="41" spans="2:2">
       <c r="B41" t="s">
         <v>34</v>
       </c>
     </row>
-    <row r="42" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="42" spans="2:2">
       <c r="B42" t="s">
         <v>35</v>
       </c>
     </row>
-    <row r="43" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="43" spans="2:2">
       <c r="B43" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="44" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="44" spans="2:2">
       <c r="B44" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="45" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="45" spans="2:2">
       <c r="B45" t="s">
         <v>38</v>
       </c>
     </row>
-    <row r="46" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:2">
       <c r="B46" t="s">
         <v>39</v>
       </c>
     </row>
-    <row r="47" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="47" spans="2:2">
       <c r="B47" t="s">
         <v>40</v>
       </c>
     </row>
-    <row r="48" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="48" spans="2:2">
       <c r="B48" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="49" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="49" spans="1:17">
       <c r="B49" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="51" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:17">
       <c r="A51" s="1"/>
       <c r="B51" s="1"/>
       <c r="C51" s="1"/>
@@ -1045,7 +1428,7 @@
       <c r="P51" s="1"/>
       <c r="Q51" s="1"/>
     </row>
-    <row r="53" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:17">
       <c r="B53" t="s">
         <v>43</v>
       </c>
@@ -1059,12 +1442,12 @@
         <v>79</v>
       </c>
     </row>
-    <row r="55" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="55" spans="1:17">
       <c r="B55" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="56" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:17">
       <c r="B56" t="s">
         <v>1</v>
       </c>
@@ -1072,7 +1455,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="57" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:17">
       <c r="B57" t="s">
         <v>3</v>
       </c>
@@ -1080,7 +1463,7 @@
         <v>47</v>
       </c>
     </row>
-    <row r="58" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="58" spans="1:17">
       <c r="B58" t="s">
         <v>5</v>
       </c>
@@ -1088,192 +1471,192 @@
         <v>48</v>
       </c>
     </row>
-    <row r="59" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:17">
       <c r="B59" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="62" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:17">
       <c r="B62" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="63" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:17">
       <c r="B63" t="s">
         <v>49</v>
       </c>
     </row>
-    <row r="64" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:17">
       <c r="B64" t="s">
         <v>50</v>
       </c>
     </row>
-    <row r="65" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="65" spans="2:2">
       <c r="B65" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="66" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="66" spans="2:2">
       <c r="B66" t="s">
         <v>52</v>
       </c>
     </row>
-    <row r="67" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="67" spans="2:2">
       <c r="B67" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="70" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="70" spans="2:2">
       <c r="B70" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="71" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="71" spans="2:2">
       <c r="B71" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="72" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="72" spans="2:2">
       <c r="B72" t="s">
         <v>53</v>
       </c>
     </row>
-    <row r="73" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="73" spans="2:2">
       <c r="B73" t="s">
         <v>54</v>
       </c>
     </row>
-    <row r="74" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="74" spans="2:2">
       <c r="B74" t="s">
         <v>55</v>
       </c>
     </row>
-    <row r="75" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="75" spans="2:2">
       <c r="B75" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="76" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="76" spans="2:2">
       <c r="B76" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="77" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="77" spans="2:2">
       <c r="B77" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="78" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="78" spans="2:2">
       <c r="B78" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="79" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="79" spans="2:2">
       <c r="B79" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="80" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="80" spans="2:2">
       <c r="B80" t="s">
         <v>61</v>
       </c>
     </row>
-    <row r="81" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="81" spans="2:2">
       <c r="B81" t="s">
         <v>62</v>
       </c>
     </row>
-    <row r="82" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="82" spans="2:2">
       <c r="B82" t="s">
         <v>63</v>
       </c>
     </row>
-    <row r="83" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="83" spans="2:2">
       <c r="B83" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="84" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="84" spans="2:2">
       <c r="B84" t="s">
         <v>65</v>
       </c>
     </row>
-    <row r="85" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="85" spans="2:2">
       <c r="B85" t="s">
         <v>66</v>
       </c>
     </row>
-    <row r="86" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="86" spans="2:2">
       <c r="B86" t="s">
         <v>67</v>
       </c>
     </row>
-    <row r="87" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="87" spans="2:2">
       <c r="B87" t="s">
         <v>68</v>
       </c>
     </row>
-    <row r="88" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="88" spans="2:2">
       <c r="B88" t="s">
         <v>69</v>
       </c>
     </row>
-    <row r="89" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="89" spans="2:2">
       <c r="B89" t="s">
         <v>70</v>
       </c>
     </row>
-    <row r="90" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="90" spans="2:2">
       <c r="B90" t="s">
         <v>71</v>
       </c>
     </row>
-    <row r="91" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="91" spans="2:2">
       <c r="B91" t="s">
         <v>72</v>
       </c>
     </row>
-    <row r="92" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="92" spans="2:2">
       <c r="B92" t="s">
         <v>73</v>
       </c>
     </row>
-    <row r="93" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="93" spans="2:2">
       <c r="B93" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="94" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="94" spans="2:2">
       <c r="B94" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="95" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="95" spans="2:2">
       <c r="B95" t="s">
         <v>76</v>
       </c>
     </row>
-    <row r="96" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="96" spans="2:2">
       <c r="B96" t="s">
         <v>77</v>
       </c>
     </row>
-    <row r="97" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="97" spans="1:17">
       <c r="B97" t="s">
         <v>78</v>
       </c>
     </row>
-    <row r="98" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="98" spans="1:17">
       <c r="B98" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="99" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="99" spans="1:17">
       <c r="B99" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="101" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="101" spans="1:17">
       <c r="A101" s="1"/>
       <c r="B101" s="1"/>
       <c r="C101" s="1"/>
@@ -1292,7 +1675,7 @@
       <c r="P101" s="1"/>
       <c r="Q101" s="1"/>
     </row>
-    <row r="103" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="103" spans="1:17">
       <c r="B103" t="s">
         <v>112</v>
       </c>
@@ -1306,17 +1689,17 @@
         <v>114</v>
       </c>
     </row>
-    <row r="104" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="104" spans="1:17">
       <c r="G104" t="s">
         <v>115</v>
       </c>
     </row>
-    <row r="105" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="105" spans="1:17">
       <c r="B105" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="106" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="106" spans="1:17">
       <c r="B106" t="s">
         <v>1</v>
       </c>
@@ -1324,7 +1707,7 @@
         <v>80</v>
       </c>
     </row>
-    <row r="107" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="107" spans="1:17">
       <c r="B107" t="s">
         <v>3</v>
       </c>
@@ -1332,7 +1715,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="108" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="108" spans="1:17">
       <c r="B108" t="s">
         <v>5</v>
       </c>
@@ -1340,188 +1723,892 @@
         <v>82</v>
       </c>
     </row>
-    <row r="109" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="109" spans="1:17">
       <c r="B109" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="112" spans="1:17" x14ac:dyDescent="0.25">
+    <row r="112" spans="1:17">
       <c r="B112" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="113" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="113" spans="2:2">
       <c r="B113" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="114" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="114" spans="2:2">
       <c r="B114" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="115" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="115" spans="2:2">
       <c r="B115" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="116" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="116" spans="2:2">
       <c r="B116" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="117" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="117" spans="2:2">
       <c r="B117" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="120" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="120" spans="2:2">
       <c r="B120" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="121" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="121" spans="2:2">
       <c r="B121" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="122" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="122" spans="2:2">
       <c r="B122" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="123" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="123" spans="2:2">
       <c r="B123" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="124" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="124" spans="2:2">
       <c r="B124" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="125" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="125" spans="2:2">
       <c r="B125" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="126" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="126" spans="2:2">
       <c r="B126" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="127" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="127" spans="2:2">
       <c r="B127" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="128" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="128" spans="2:2">
       <c r="B128" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="129" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="129" spans="2:2">
       <c r="B129" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="130" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="130" spans="2:2">
       <c r="B130" t="s">
         <v>94</v>
       </c>
     </row>
-    <row r="131" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="131" spans="2:2">
       <c r="B131" t="s">
         <v>95</v>
       </c>
     </row>
-    <row r="132" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="132" spans="2:2">
       <c r="B132" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="133" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="133" spans="2:2">
       <c r="B133" t="s">
         <v>97</v>
       </c>
     </row>
-    <row r="134" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="134" spans="2:2">
       <c r="B134" t="s">
         <v>98</v>
       </c>
     </row>
-    <row r="135" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="135" spans="2:2">
       <c r="B135" t="s">
         <v>99</v>
       </c>
     </row>
-    <row r="136" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="136" spans="2:2">
       <c r="B136" t="s">
         <v>100</v>
       </c>
     </row>
-    <row r="137" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="137" spans="2:2">
       <c r="B137" t="s">
         <v>101</v>
       </c>
     </row>
-    <row r="138" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="138" spans="2:2">
       <c r="B138" t="s">
         <v>102</v>
       </c>
     </row>
-    <row r="139" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="139" spans="2:2">
       <c r="B139" t="s">
         <v>103</v>
       </c>
     </row>
-    <row r="140" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="140" spans="2:2">
       <c r="B140" t="s">
         <v>104</v>
       </c>
     </row>
-    <row r="141" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="141" spans="2:2">
       <c r="B141" t="s">
         <v>105</v>
       </c>
     </row>
-    <row r="142" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="142" spans="2:2">
       <c r="B142" t="s">
         <v>106</v>
       </c>
     </row>
-    <row r="143" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="143" spans="2:2">
       <c r="B143" t="s">
         <v>107</v>
       </c>
     </row>
-    <row r="144" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="144" spans="2:2">
       <c r="B144" t="s">
         <v>108</v>
       </c>
     </row>
-    <row r="145" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="145" spans="1:17">
       <c r="B145" t="s">
         <v>109</v>
       </c>
     </row>
-    <row r="146" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="146" spans="1:17">
       <c r="B146" t="s">
         <v>110</v>
       </c>
     </row>
-    <row r="147" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="147" spans="1:17">
       <c r="B147" t="s">
         <v>111</v>
       </c>
     </row>
-    <row r="148" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="148" spans="1:17">
       <c r="B148" t="s">
         <v>41</v>
       </c>
     </row>
-    <row r="149" spans="2:2" x14ac:dyDescent="0.25">
+    <row r="149" spans="1:17">
       <c r="B149" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="151" spans="1:17">
+      <c r="A151" s="1"/>
+      <c r="B151" s="1"/>
+      <c r="C151" s="1"/>
+      <c r="D151" s="1"/>
+      <c r="E151" s="1"/>
+      <c r="F151" s="1"/>
+      <c r="G151" s="1"/>
+      <c r="H151" s="1"/>
+      <c r="I151" s="1"/>
+      <c r="J151" s="1"/>
+      <c r="K151" s="1"/>
+      <c r="L151" s="1"/>
+      <c r="M151" s="1"/>
+      <c r="N151" s="1"/>
+      <c r="O151" s="1"/>
+      <c r="P151" s="1"/>
+      <c r="Q151" s="1"/>
+    </row>
+    <row r="155" spans="1:17">
+      <c r="B155" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="156" spans="1:17">
+      <c r="B156" t="s">
+        <v>1</v>
+      </c>
+      <c r="E156" t="s">
+        <v>116</v>
+      </c>
+    </row>
+    <row r="157" spans="1:17">
+      <c r="B157" t="s">
+        <v>3</v>
+      </c>
+      <c r="D157" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="158" spans="1:17">
+      <c r="B158" t="s">
+        <v>5</v>
+      </c>
+      <c r="C158" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="159" spans="1:17">
+      <c r="B159" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="162" spans="2:2">
+      <c r="B162" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="163" spans="2:2">
+      <c r="B163" t="s">
+        <v>119</v>
+      </c>
+    </row>
+    <row r="164" spans="2:2">
+      <c r="B164" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="165" spans="2:2">
+      <c r="B165" t="s">
+        <v>121</v>
+      </c>
+    </row>
+    <row r="166" spans="2:2">
+      <c r="B166" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="167" spans="2:2">
+      <c r="B167" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="170" spans="2:2">
+      <c r="B170" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="171" spans="2:2">
+      <c r="B171" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="172" spans="2:2">
+      <c r="B172" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="173" spans="2:2">
+      <c r="B173" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="174" spans="2:2">
+      <c r="B174" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="175" spans="2:2">
+      <c r="B175" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="176" spans="2:2">
+      <c r="B176" t="s">
+        <v>125</v>
+      </c>
+    </row>
+    <row r="177" spans="2:2">
+      <c r="B177" t="s">
+        <v>126</v>
+      </c>
+    </row>
+    <row r="178" spans="2:2">
+      <c r="B178" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="179" spans="2:2">
+      <c r="B179" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="180" spans="2:2">
+      <c r="B180" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="181" spans="2:2">
+      <c r="B181" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="182" spans="2:2">
+      <c r="B182" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="183" spans="2:2">
+      <c r="B183" t="s">
+        <v>132</v>
+      </c>
+    </row>
+    <row r="184" spans="2:2">
+      <c r="B184" t="s">
+        <v>133</v>
+      </c>
+    </row>
+    <row r="185" spans="2:2">
+      <c r="B185" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="186" spans="2:2">
+      <c r="B186" t="s">
+        <v>135</v>
+      </c>
+    </row>
+    <row r="187" spans="2:2">
+      <c r="B187" t="s">
+        <v>136</v>
+      </c>
+    </row>
+    <row r="188" spans="2:2">
+      <c r="B188" t="s">
+        <v>137</v>
+      </c>
+    </row>
+    <row r="189" spans="2:2">
+      <c r="B189" t="s">
+        <v>138</v>
+      </c>
+    </row>
+    <row r="190" spans="2:2">
+      <c r="B190" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="191" spans="2:2">
+      <c r="B191" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="192" spans="2:2">
+      <c r="B192" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="193" spans="1:17">
+      <c r="B193" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="194" spans="1:17">
+      <c r="B194" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="195" spans="1:17">
+      <c r="B195" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="196" spans="1:17">
+      <c r="B196" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="197" spans="1:17">
+      <c r="B197" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="198" spans="1:17">
+      <c r="B198" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="199" spans="1:17">
+      <c r="B199" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="201" spans="1:17">
+      <c r="A201" s="1"/>
+      <c r="B201" s="1"/>
+      <c r="C201" s="1"/>
+      <c r="D201" s="1"/>
+      <c r="E201" s="1"/>
+      <c r="F201" s="1"/>
+      <c r="G201" s="1"/>
+      <c r="H201" s="1"/>
+      <c r="I201" s="1"/>
+      <c r="J201" s="1"/>
+      <c r="K201" s="1"/>
+      <c r="L201" s="1"/>
+      <c r="M201" s="1"/>
+      <c r="N201" s="1"/>
+      <c r="O201" s="1"/>
+      <c r="P201" s="1"/>
+      <c r="Q201" s="1"/>
+    </row>
+    <row r="205" spans="1:17">
+      <c r="B205" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="206" spans="1:17">
+      <c r="B206" t="s">
+        <v>1</v>
+      </c>
+      <c r="E206" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="207" spans="1:17">
+      <c r="B207" t="s">
+        <v>3</v>
+      </c>
+      <c r="D207" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="208" spans="1:17">
+      <c r="B208" t="s">
+        <v>5</v>
+      </c>
+      <c r="C208" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="209" spans="2:2">
+      <c r="B209" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="212" spans="2:2">
+      <c r="B212" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="213" spans="2:2">
+      <c r="B213" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="214" spans="2:2">
+      <c r="B214" t="s">
+        <v>151</v>
+      </c>
+    </row>
+    <row r="215" spans="2:2">
+      <c r="B215" t="s">
+        <v>152</v>
+      </c>
+    </row>
+    <row r="216" spans="2:2">
+      <c r="B216" t="s">
+        <v>153</v>
+      </c>
+    </row>
+    <row r="217" spans="2:2">
+      <c r="B217" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="220" spans="2:2">
+      <c r="B220" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="221" spans="2:2">
+      <c r="B221" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="222" spans="2:2">
+      <c r="B222" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="223" spans="2:2">
+      <c r="B223" t="s">
+        <v>154</v>
+      </c>
+    </row>
+    <row r="224" spans="2:2">
+      <c r="B224" t="s">
+        <v>155</v>
+      </c>
+    </row>
+    <row r="225" spans="2:2">
+      <c r="B225" t="s">
+        <v>156</v>
+      </c>
+    </row>
+    <row r="226" spans="2:2">
+      <c r="B226" t="s">
+        <v>157</v>
+      </c>
+    </row>
+    <row r="227" spans="2:2">
+      <c r="B227" t="s">
+        <v>158</v>
+      </c>
+    </row>
+    <row r="228" spans="2:2">
+      <c r="B228" t="s">
+        <v>159</v>
+      </c>
+    </row>
+    <row r="229" spans="2:2">
+      <c r="B229" t="s">
+        <v>160</v>
+      </c>
+    </row>
+    <row r="230" spans="2:2">
+      <c r="B230" t="s">
+        <v>161</v>
+      </c>
+    </row>
+    <row r="231" spans="2:2">
+      <c r="B231" t="s">
+        <v>162</v>
+      </c>
+    </row>
+    <row r="232" spans="2:2">
+      <c r="B232" t="s">
+        <v>163</v>
+      </c>
+    </row>
+    <row r="233" spans="2:2">
+      <c r="B233" t="s">
+        <v>164</v>
+      </c>
+    </row>
+    <row r="234" spans="2:2">
+      <c r="B234" t="s">
+        <v>165</v>
+      </c>
+    </row>
+    <row r="235" spans="2:2">
+      <c r="B235" t="s">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="236" spans="2:2">
+      <c r="B236" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="237" spans="2:2">
+      <c r="B237" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="238" spans="2:2">
+      <c r="B238" t="s">
+        <v>169</v>
+      </c>
+    </row>
+    <row r="239" spans="2:2">
+      <c r="B239" t="s">
+        <v>170</v>
+      </c>
+    </row>
+    <row r="240" spans="2:2">
+      <c r="B240" t="s">
+        <v>171</v>
+      </c>
+    </row>
+    <row r="241" spans="1:17">
+      <c r="B241" t="s">
+        <v>172</v>
+      </c>
+    </row>
+    <row r="242" spans="1:17">
+      <c r="B242" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="243" spans="1:17">
+      <c r="B243" t="s">
+        <v>174</v>
+      </c>
+    </row>
+    <row r="244" spans="1:17">
+      <c r="B244" t="s">
+        <v>175</v>
+      </c>
+    </row>
+    <row r="245" spans="1:17">
+      <c r="B245" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="246" spans="1:17">
+      <c r="B246" t="s">
+        <v>176</v>
+      </c>
+    </row>
+    <row r="247" spans="1:17">
+      <c r="B247" t="s">
+        <v>177</v>
+      </c>
+    </row>
+    <row r="248" spans="1:17">
+      <c r="B248" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="249" spans="1:17">
+      <c r="B249" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="250" spans="1:17">
+      <c r="B250" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="252" spans="1:17">
+      <c r="A252" s="1"/>
+      <c r="B252" s="1"/>
+      <c r="C252" s="1"/>
+      <c r="D252" s="1"/>
+      <c r="E252" s="1"/>
+      <c r="F252" s="1"/>
+      <c r="G252" s="1"/>
+      <c r="H252" s="1"/>
+      <c r="I252" s="1"/>
+      <c r="J252" s="1"/>
+      <c r="K252" s="1"/>
+      <c r="L252" s="1"/>
+      <c r="M252" s="1"/>
+      <c r="N252" s="1"/>
+      <c r="O252" s="1"/>
+      <c r="P252" s="1"/>
+      <c r="Q252" s="1"/>
+    </row>
+    <row r="256" spans="1:17">
+      <c r="B256" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="257" spans="2:5">
+      <c r="B257" t="s">
+        <v>1</v>
+      </c>
+      <c r="E257" t="s">
+        <v>179</v>
+      </c>
+    </row>
+    <row r="258" spans="2:5">
+      <c r="B258" t="s">
+        <v>3</v>
+      </c>
+      <c r="D258" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="259" spans="2:5">
+      <c r="B259" t="s">
+        <v>5</v>
+      </c>
+      <c r="C259" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="260" spans="2:5">
+      <c r="B260" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="263" spans="2:5">
+      <c r="B263" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="264" spans="2:5">
+      <c r="B264" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="265" spans="2:5">
+      <c r="B265" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="266" spans="2:5">
+      <c r="B266" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="267" spans="2:5">
+      <c r="B267" t="s">
+        <v>185</v>
+      </c>
+    </row>
+    <row r="268" spans="2:5">
+      <c r="B268" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="271" spans="2:5">
+      <c r="B271" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="272" spans="2:5">
+      <c r="B272" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="273" spans="2:2">
+      <c r="B273" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="274" spans="2:2">
+      <c r="B274" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="275" spans="2:2">
+      <c r="B275" t="s">
+        <v>186</v>
+      </c>
+    </row>
+    <row r="276" spans="2:2">
+      <c r="B276" t="s">
+        <v>187</v>
+      </c>
+    </row>
+    <row r="277" spans="2:2">
+      <c r="B277" t="s">
+        <v>188</v>
+      </c>
+    </row>
+    <row r="278" spans="2:2">
+      <c r="B278" t="s">
+        <v>189</v>
+      </c>
+    </row>
+    <row r="279" spans="2:2">
+      <c r="B279" t="s">
+        <v>190</v>
+      </c>
+    </row>
+    <row r="280" spans="2:2">
+      <c r="B280" t="s">
+        <v>191</v>
+      </c>
+    </row>
+    <row r="281" spans="2:2">
+      <c r="B281" t="s">
+        <v>192</v>
+      </c>
+    </row>
+    <row r="282" spans="2:2">
+      <c r="B282" t="s">
+        <v>193</v>
+      </c>
+    </row>
+    <row r="283" spans="2:2">
+      <c r="B283" t="s">
+        <v>194</v>
+      </c>
+    </row>
+    <row r="284" spans="2:2">
+      <c r="B284" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="285" spans="2:2">
+      <c r="B285" t="s">
+        <v>196</v>
+      </c>
+    </row>
+    <row r="286" spans="2:2">
+      <c r="B286" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="287" spans="2:2">
+      <c r="B287" t="s">
+        <v>198</v>
+      </c>
+    </row>
+    <row r="288" spans="2:2">
+      <c r="B288" t="s">
+        <v>199</v>
+      </c>
+    </row>
+    <row r="289" spans="2:2">
+      <c r="B289" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="290" spans="2:2">
+      <c r="B290" t="s">
+        <v>201</v>
+      </c>
+    </row>
+    <row r="291" spans="2:2">
+      <c r="B291" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="292" spans="2:2">
+      <c r="B292" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="293" spans="2:2">
+      <c r="B293" t="s">
+        <v>204</v>
+      </c>
+    </row>
+    <row r="294" spans="2:2">
+      <c r="B294" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="295" spans="2:2">
+      <c r="B295" t="s">
+        <v>206</v>
+      </c>
+    </row>
+    <row r="296" spans="2:2">
+      <c r="B296" t="s">
+        <v>207</v>
+      </c>
+    </row>
+    <row r="297" spans="2:2">
+      <c r="B297" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="298" spans="2:2">
+      <c r="B298" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="299" spans="2:2">
+      <c r="B299" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="300" spans="2:2">
+      <c r="B300" t="s">
         <v>42</v>
       </c>
     </row>

</xml_diff>